<commit_message>
cleaning up validation and training files
</commit_message>
<xml_diff>
--- a/gen/output.xlsx
+++ b/gen/output.xlsx
@@ -723,7 +723,7 @@
         <v>1</v>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -767,7 +767,7 @@
         <v>1</v>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1680,7 +1680,7 @@
         <v>0</v>
       </c>
       <c r="C119" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:3">
@@ -1823,7 +1823,7 @@
         <v>1</v>
       </c>
       <c r="C132" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:3">
@@ -3308,7 +3308,7 @@
         <v>1</v>
       </c>
       <c r="C267" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268" spans="1:3">
@@ -3451,7 +3451,7 @@
         <v>0</v>
       </c>
       <c r="C280" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="281" spans="1:3">
@@ -3605,7 +3605,7 @@
         <v>0</v>
       </c>
       <c r="C294" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="295" spans="1:3">
@@ -3682,7 +3682,7 @@
         <v>1</v>
       </c>
       <c r="C301" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="302" spans="1:3">
@@ -4012,7 +4012,7 @@
         <v>0</v>
       </c>
       <c r="C331" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="332" spans="1:3">
@@ -4694,7 +4694,7 @@
         <v>1</v>
       </c>
       <c r="C393" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="394" spans="1:3">
@@ -5200,7 +5200,7 @@
         <v>0</v>
       </c>
       <c r="C439" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="440" spans="1:3">
@@ -5409,7 +5409,7 @@
         <v>1</v>
       </c>
       <c r="C458" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="459" spans="1:3">
@@ -5728,7 +5728,7 @@
         <v>1</v>
       </c>
       <c r="C487" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="488" spans="1:3">
@@ -5761,7 +5761,7 @@
         <v>0</v>
       </c>
       <c r="C490" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="491" spans="1:3">
@@ -5860,7 +5860,7 @@
         <v>1</v>
       </c>
       <c r="C499" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="500" spans="1:3">
@@ -6542,7 +6542,7 @@
         <v>1</v>
       </c>
       <c r="C561" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="562" spans="1:3">
@@ -6916,7 +6916,7 @@
         <v>1</v>
       </c>
       <c r="C595" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="596" spans="1:3">
@@ -7147,7 +7147,7 @@
         <v>1</v>
       </c>
       <c r="C616" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="617" spans="1:3">
@@ -7158,7 +7158,7 @@
         <v>1</v>
       </c>
       <c r="C617" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="618" spans="1:3">
@@ -8489,7 +8489,7 @@
         <v>1</v>
       </c>
       <c r="C738" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="739" spans="1:3">
@@ -8555,7 +8555,7 @@
         <v>1</v>
       </c>
       <c r="C744" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="745" spans="1:3">
@@ -8720,7 +8720,7 @@
         <v>0</v>
       </c>
       <c r="C759" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="760" spans="1:3">
@@ -9138,7 +9138,7 @@
         <v>0</v>
       </c>
       <c r="C797" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="798" spans="1:3">
@@ -9721,7 +9721,7 @@
         <v>0</v>
       </c>
       <c r="C850" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="851" spans="1:3">
@@ -9842,7 +9842,7 @@
         <v>0</v>
       </c>
       <c r="C861" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="862" spans="1:3">
@@ -10073,7 +10073,7 @@
         <v>1</v>
       </c>
       <c r="C882" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="883" spans="1:3">
@@ -10106,7 +10106,7 @@
         <v>0</v>
       </c>
       <c r="C885" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="886" spans="1:3">
@@ -10491,7 +10491,7 @@
         <v>1</v>
       </c>
       <c r="C920" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="921" spans="1:3">
@@ -10766,7 +10766,7 @@
         <v>1</v>
       </c>
       <c r="C945" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="946" spans="1:3">
@@ -10975,7 +10975,7 @@
         <v>1</v>
       </c>
       <c r="C964" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="965" spans="1:3">
@@ -11415,7 +11415,7 @@
         <v>0</v>
       </c>
       <c r="C1004" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1005" spans="1:3">
@@ -12471,7 +12471,7 @@
         <v>1</v>
       </c>
       <c r="C1100" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1101" spans="1:3">
@@ -12669,7 +12669,7 @@
         <v>0</v>
       </c>
       <c r="C1118" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1119" spans="1:3">
@@ -12911,7 +12911,7 @@
         <v>0</v>
       </c>
       <c r="C1140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1141" spans="1:3">
@@ -12922,7 +12922,7 @@
         <v>1</v>
       </c>
       <c r="C1141" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1142" spans="1:3">
@@ -13593,7 +13593,7 @@
         <v>1</v>
       </c>
       <c r="C1202" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1203" spans="1:3">
@@ -13736,7 +13736,7 @@
         <v>1</v>
       </c>
       <c r="C1215" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1216" spans="1:3">
@@ -14022,7 +14022,7 @@
         <v>1</v>
       </c>
       <c r="C1241" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1242" spans="1:3">
@@ -14143,7 +14143,7 @@
         <v>0</v>
       </c>
       <c r="C1252" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1253" spans="1:3">
@@ -14429,7 +14429,7 @@
         <v>1</v>
       </c>
       <c r="C1278" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1279" spans="1:3">
@@ -14605,7 +14605,7 @@
         <v>1</v>
       </c>
       <c r="C1294" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1295" spans="1:3">
@@ -14924,7 +14924,7 @@
         <v>1</v>
       </c>
       <c r="C1323" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1324" spans="1:3">
@@ -15012,7 +15012,7 @@
         <v>0</v>
       </c>
       <c r="C1331" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1332" spans="1:3">
@@ -15463,7 +15463,7 @@
         <v>0</v>
       </c>
       <c r="C1372" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1373" spans="1:3">
@@ -17267,7 +17267,7 @@
         <v>0</v>
       </c>
       <c r="C1536" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1537" spans="1:3">
@@ -17509,7 +17509,7 @@
         <v>1</v>
       </c>
       <c r="C1558" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1559" spans="1:3">
@@ -17795,7 +17795,7 @@
         <v>0</v>
       </c>
       <c r="C1584" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1585" spans="1:3">
@@ -18785,7 +18785,7 @@
         <v>1</v>
       </c>
       <c r="C1674" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1675" spans="1:3">
@@ -18939,7 +18939,7 @@
         <v>1</v>
       </c>
       <c r="C1688" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1689" spans="1:3">
@@ -19126,7 +19126,7 @@
         <v>0</v>
       </c>
       <c r="C1705" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1706" spans="1:3">
@@ -19544,7 +19544,7 @@
         <v>1</v>
       </c>
       <c r="C1743" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1744" spans="1:3">
@@ -19786,7 +19786,7 @@
         <v>1</v>
       </c>
       <c r="C1765" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1766" spans="1:3">
@@ -20545,7 +20545,7 @@
         <v>1</v>
       </c>
       <c r="C1834" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1835" spans="1:3">
@@ -20754,7 +20754,7 @@
         <v>1</v>
       </c>
       <c r="C1853" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1854" spans="1:3">
@@ -21205,7 +21205,7 @@
         <v>1</v>
       </c>
       <c r="C1894" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="1895" spans="1:3">
@@ -21447,7 +21447,7 @@
         <v>1</v>
       </c>
       <c r="C1916" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="1917" spans="1:3">

</xml_diff>